<commit_message>
Redid SSAO measurements as they were skewed
</commit_message>
<xml_diff>
--- a/Experiment/Results/Framerate.xlsx
+++ b/Experiment/Results/Framerate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Howest\GD_J3_S2\Gradwork_2.0\Gradwork\Experiment\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E705543-49F7-489E-87E2-98F54A9CD1A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5126D3D8-BF02-4318-A51E-BF97FC04E3A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19580" yWindow="-9330" windowWidth="17940" windowHeight="10660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22260" yWindow="-10390" windowWidth="16430" windowHeight="12340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SSAO" sheetId="1" r:id="rId1"/>
@@ -569,8 +569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:X15"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U17" sqref="T17:U17"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X16" sqref="X16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -579,13 +579,13 @@
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
     <col min="15" max="18" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
     <col min="20" max="24" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -674,67 +674,67 @@
       </c>
       <c r="D4" s="12">
         <f>AVERAGE(E4:AC4)</f>
-        <v>0.44409919999999986</v>
+        <v>0.17290160000000002</v>
       </c>
       <c r="E4" s="12">
-        <v>0.61849600000000005</v>
+        <v>8.7040000000000006E-2</v>
       </c>
       <c r="F4" s="12">
-        <v>0.43827199999999999</v>
+        <v>0.65228799999999998</v>
       </c>
       <c r="G4" s="12">
-        <v>0.735232</v>
+        <v>0.24268799999999999</v>
       </c>
       <c r="H4" s="12">
-        <v>0.32256000000000001</v>
+        <v>9.2160000000000006E-2</v>
       </c>
       <c r="I4" s="12">
-        <v>0.58320000000000005</v>
+        <v>8.7040000000000006E-2</v>
       </c>
       <c r="J4" s="12">
-        <v>0.63590400000000002</v>
+        <v>9.1120000000000007E-2</v>
       </c>
       <c r="K4" s="12">
-        <v>0.31539200000000001</v>
+        <v>0.25292799999999999</v>
       </c>
       <c r="L4" s="12">
-        <v>2.3705599999999998</v>
+        <v>8.4991999999999998E-2</v>
       </c>
       <c r="M4" s="12">
-        <v>8.3968000000000001E-2</v>
+        <v>8.7040000000000006E-2</v>
       </c>
       <c r="N4" s="12">
-        <v>8.0895999999999996E-2</v>
+        <v>8.7040000000000006E-2</v>
       </c>
       <c r="O4" s="12">
-        <v>0.694272</v>
+        <v>0.90726399999999996</v>
       </c>
       <c r="P4" s="12">
+        <v>9.0111999999999998E-2</v>
+      </c>
+      <c r="Q4" s="12">
+        <v>8.1920000000000007E-2</v>
+      </c>
+      <c r="R4" s="12">
+        <v>9.0111999999999998E-2</v>
+      </c>
+      <c r="S4" s="12">
+        <v>8.8064000000000003E-2</v>
+      </c>
+      <c r="T4" s="12">
+        <v>8.9088000000000001E-2</v>
+      </c>
+      <c r="U4" s="12">
+        <v>8.8064000000000003E-2</v>
+      </c>
+      <c r="V4" s="12">
         <v>8.6015999999999995E-2</v>
       </c>
-      <c r="Q4" s="12">
-        <v>9.1135999999999995E-2</v>
-      </c>
-      <c r="R4" s="12">
-        <v>9.1135999999999995E-2</v>
-      </c>
-      <c r="S4" s="12">
-        <v>8.0159999999999995E-2</v>
-      </c>
-      <c r="T4" s="12">
-        <v>0.67379199999999995</v>
-      </c>
-      <c r="U4" s="12">
-        <v>8.9088000000000001E-2</v>
-      </c>
-      <c r="V4" s="12">
-        <v>0.71679999999999999</v>
-      </c>
       <c r="W4" s="11">
-        <v>8.7040000000000006E-2</v>
+        <v>9.0111999999999998E-2</v>
       </c>
       <c r="X4" s="12">
-        <v>8.8064000000000003E-2</v>
+        <v>8.2944000000000004E-2</v>
       </c>
     </row>
     <row r="5" spans="2:24" x14ac:dyDescent="0.3">
@@ -746,67 +746,67 @@
       </c>
       <c r="D5" s="12">
         <f t="shared" ref="D5:D15" si="0">AVERAGE(E5:AC5)</f>
-        <v>1.5683584000000004</v>
+        <v>0.55299875000000009</v>
       </c>
       <c r="E5" s="15">
-        <v>2.03776</v>
+        <v>0.31948799999999999</v>
       </c>
       <c r="F5" s="15">
-        <v>3.0095360000000002</v>
+        <v>0.31436799999999998</v>
       </c>
       <c r="G5" s="15">
-        <v>1.1632640000000001</v>
+        <v>0.86118399999999995</v>
       </c>
       <c r="H5" s="15">
-        <v>10.340351999999999</v>
+        <v>0.32972800000000002</v>
       </c>
       <c r="I5" s="15">
-        <v>2.650112</v>
+        <v>0.31072699999999998</v>
       </c>
       <c r="J5" s="15">
-        <v>2.3193600000000001</v>
+        <v>0.33823999999999999</v>
       </c>
       <c r="K5" s="15">
-        <v>2.656256</v>
+        <v>0.32358399999999998</v>
       </c>
       <c r="L5" s="15">
-        <v>1.4643200000000001</v>
+        <v>0.31129600000000002</v>
       </c>
       <c r="M5" s="15">
         <v>0.32051200000000002</v>
       </c>
       <c r="N5" s="15">
-        <v>0.31027199999999999</v>
+        <v>0.31641599999999998</v>
       </c>
       <c r="O5" s="15">
-        <v>0.31948799999999999</v>
+        <v>0.32153599999999999</v>
       </c>
       <c r="P5" s="15">
-        <v>0.31948799999999999</v>
+        <v>0.69017600000000001</v>
       </c>
       <c r="Q5" s="15">
-        <v>0.33075199999999999</v>
+        <v>0.30310399999999998</v>
       </c>
       <c r="R5" s="15">
-        <v>0.326656</v>
+        <v>4.0857599999999996</v>
       </c>
       <c r="S5" s="15">
-        <v>0.31436799999999998</v>
+        <v>0.32153599999999999</v>
       </c>
       <c r="T5" s="15">
-        <v>0.326656</v>
+        <v>0.32768000000000003</v>
       </c>
       <c r="U5" s="15">
-        <v>0.32460800000000001</v>
+        <v>0.32051200000000002</v>
       </c>
       <c r="V5" s="15">
-        <v>0.31334400000000001</v>
+        <v>0.31846400000000002</v>
       </c>
       <c r="W5" s="14">
-        <v>0.32358399999999998</v>
+        <v>0.31641599999999998</v>
       </c>
       <c r="X5" s="15">
-        <v>2.1964800000000002</v>
+        <v>0.30924800000000002</v>
       </c>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.3">
@@ -818,67 +818,67 @@
       </c>
       <c r="D6" s="12">
         <f t="shared" si="0"/>
-        <v>3.1878136000000006</v>
+        <v>1.8796544000000004</v>
       </c>
       <c r="E6" s="15">
-        <v>13.139968</v>
+        <v>2.911232</v>
       </c>
       <c r="F6" s="15">
-        <v>1.41726</v>
+        <v>1.3209599999999999</v>
       </c>
       <c r="G6" s="15">
-        <v>11.983872</v>
+        <v>5.1558400000000004</v>
       </c>
       <c r="H6" s="15">
-        <v>1.422336</v>
+        <v>1.499136</v>
       </c>
       <c r="I6" s="15">
-        <v>2.5333760000000001</v>
+        <v>1.3926400000000001</v>
       </c>
       <c r="J6" s="15">
-        <v>5.4958080000000002</v>
+        <v>1.4213119999999999</v>
       </c>
       <c r="K6" s="15">
+        <v>1.3926400000000001</v>
+      </c>
+      <c r="L6" s="15">
+        <v>1.2124159999999999</v>
+      </c>
+      <c r="M6" s="15">
+        <v>1.4530559999999999</v>
+      </c>
+      <c r="N6" s="15">
+        <v>3.4815999999999998</v>
+      </c>
+      <c r="O6" s="15">
+        <v>1.3557760000000001</v>
+      </c>
+      <c r="P6" s="15">
+        <v>1.4745600000000001</v>
+      </c>
+      <c r="Q6" s="15">
+        <v>1.301504</v>
+      </c>
+      <c r="R6" s="15">
         <v>1.333248</v>
       </c>
-      <c r="L6" s="15">
-        <v>8.4971519999999998</v>
-      </c>
-      <c r="M6" s="15">
-        <v>1.272832</v>
-      </c>
-      <c r="N6" s="15">
-        <v>1.293312</v>
-      </c>
-      <c r="O6" s="15">
-        <v>1.44896</v>
-      </c>
-      <c r="P6" s="15">
-        <v>1.296384</v>
-      </c>
-      <c r="Q6" s="15">
-        <v>1.5482279999999999</v>
-      </c>
-      <c r="R6" s="15">
-        <v>1.5165439999999999</v>
-      </c>
       <c r="S6" s="15">
-        <v>2.5876480000000002</v>
+        <v>1.4295040000000001</v>
       </c>
       <c r="T6" s="15">
-        <v>1.512448</v>
+        <v>1.528832</v>
       </c>
       <c r="U6" s="15">
-        <v>1.2605440000000001</v>
+        <v>1.2902400000000001</v>
       </c>
       <c r="V6" s="15">
-        <v>1.4213119999999999</v>
+        <v>3.8215680000000001</v>
       </c>
       <c r="W6" s="14">
-        <v>1.271808</v>
+        <v>1.435648</v>
       </c>
       <c r="X6" s="15">
-        <v>1.5032319999999999</v>
+        <v>1.3813759999999999</v>
       </c>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.3">
@@ -890,67 +890,67 @@
       </c>
       <c r="D7" s="3">
         <f t="shared" si="0"/>
-        <v>0.51292543999999995</v>
+        <v>0.47689280000000006</v>
       </c>
       <c r="E7" s="6">
-        <v>1.3895679999999999</v>
+        <v>0.31846400000000002</v>
       </c>
       <c r="F7" s="6">
-        <v>0.33823999999999999</v>
+        <v>0.33382400000000001</v>
       </c>
       <c r="G7" s="6">
-        <v>0.356352</v>
+        <v>0.32460800000000001</v>
       </c>
       <c r="H7" s="6">
-        <v>0.335872</v>
+        <v>0.34508800000000001</v>
       </c>
       <c r="I7" s="6">
-        <v>0.34406399999999998</v>
+        <v>0.33894400000000002</v>
       </c>
       <c r="J7" s="6">
-        <v>0.33075199999999999</v>
+        <v>0.32460800000000001</v>
       </c>
       <c r="K7" s="6">
         <v>0.326656</v>
       </c>
       <c r="L7" s="6">
-        <v>0.34201599999999999</v>
+        <v>0.33894400000000002</v>
       </c>
       <c r="M7" s="6">
-        <v>0.335872</v>
+        <v>0.34406399999999998</v>
       </c>
       <c r="N7" s="6">
-        <v>1.1189887999999999</v>
+        <v>0.48742400000000002</v>
       </c>
       <c r="O7" s="6">
-        <v>0.33382400000000001</v>
+        <v>0.33894400000000002</v>
       </c>
       <c r="P7" s="6">
-        <v>0.33484799999999998</v>
+        <v>0.34099200000000002</v>
       </c>
       <c r="Q7" s="6">
-        <v>0.33792</v>
+        <v>1.206272</v>
       </c>
       <c r="R7" s="6">
-        <v>0.33177600000000002</v>
+        <v>1.7827839999999999</v>
       </c>
       <c r="S7" s="6">
-        <v>0.33075199999999999</v>
+        <v>0.33689599999999997</v>
       </c>
       <c r="T7" s="6">
-        <v>0.33279999999999998</v>
+        <v>0.33823999999999999</v>
       </c>
       <c r="U7" s="6">
-        <v>0.335872</v>
+        <v>0.33996799999999999</v>
       </c>
       <c r="V7" s="6">
         <v>0.33484799999999998</v>
       </c>
       <c r="W7" s="5">
-        <v>0.335872</v>
+        <v>0.49971199999999999</v>
       </c>
       <c r="X7" s="6">
-        <v>2.0316160000000001</v>
+        <v>0.53657600000000005</v>
       </c>
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.3">
@@ -962,67 +962,67 @@
       </c>
       <c r="D8" s="3">
         <f t="shared" si="0"/>
-        <v>63.539381000000013</v>
+        <v>1.6642559999999995</v>
       </c>
       <c r="E8" s="6">
-        <v>2.54304</v>
+        <v>1.1991039999999999</v>
       </c>
       <c r="F8" s="6">
+        <v>1.2257279999999999</v>
+      </c>
+      <c r="G8" s="6">
+        <v>1.2072959999999999</v>
+      </c>
+      <c r="H8" s="6">
+        <v>1.2451840000000001</v>
+      </c>
+      <c r="I8" s="6">
+        <v>7.8202879999999997</v>
+      </c>
+      <c r="J8" s="6">
+        <v>1.2032</v>
+      </c>
+      <c r="K8" s="6">
+        <v>1.211392</v>
+      </c>
+      <c r="L8" s="6">
+        <v>1.227776</v>
+      </c>
+      <c r="M8" s="6">
+        <v>1.25952</v>
+      </c>
+      <c r="N8" s="6">
+        <v>1.9097599999999999</v>
+      </c>
+      <c r="O8" s="6">
+        <v>1.2236800000000001</v>
+      </c>
+      <c r="P8" s="6">
+        <v>1.234944</v>
+      </c>
+      <c r="Q8" s="6">
+        <v>1.77152</v>
+      </c>
+      <c r="R8" s="6">
+        <v>1.2083200000000001</v>
+      </c>
+      <c r="S8" s="6">
         <v>1.2308479999999999</v>
       </c>
-      <c r="G8" s="6">
-        <v>1.2369920000000001</v>
-      </c>
-      <c r="H8" s="6">
-        <v>1.2472319999999999</v>
-      </c>
-      <c r="I8" s="6">
-        <v>4.2649600000000003</v>
-      </c>
-      <c r="J8" s="6">
-        <v>1.328128</v>
-      </c>
-      <c r="K8" s="6">
-        <v>4.7554559999999997</v>
-      </c>
-      <c r="L8" s="6">
-        <v>1.6588799999999999</v>
-      </c>
-      <c r="M8" s="6">
-        <v>1.246208</v>
-      </c>
-      <c r="N8" s="6">
-        <v>1.2083200000000001</v>
-      </c>
-      <c r="O8" s="6">
-        <v>1.2308479999999999</v>
-      </c>
-      <c r="P8" s="6">
-        <v>1.2216320000000001</v>
-      </c>
-      <c r="Q8" s="6">
-        <v>1.2236800000000001</v>
-      </c>
-      <c r="R8" s="6">
-        <v>1239.04</v>
-      </c>
-      <c r="S8" s="6">
-        <v>1.2267520000000001</v>
-      </c>
       <c r="T8" s="6">
-        <v>1.2258279999999999</v>
+        <v>1.2206079999999999</v>
       </c>
       <c r="U8" s="6">
-        <v>1.2400640000000001</v>
+        <v>1.2339199999999999</v>
       </c>
       <c r="V8" s="6">
-        <v>1.224704</v>
+        <v>1.2390399999999999</v>
       </c>
       <c r="W8" s="5">
-        <v>1.216512</v>
+        <v>1.5400959999999999</v>
       </c>
       <c r="X8" s="6">
-        <v>1.217536</v>
+        <v>1.8728959999999999</v>
       </c>
     </row>
     <row r="9" spans="2:24" x14ac:dyDescent="0.3">
@@ -1034,67 +1034,67 @@
       </c>
       <c r="D9" s="3">
         <f t="shared" si="0"/>
-        <v>6.2810214400000008</v>
+        <v>5.3187177999999999</v>
       </c>
       <c r="E9" s="6">
-        <v>5.3227520000000004</v>
+        <v>4.8824319999999997</v>
       </c>
       <c r="F9" s="6">
-        <v>5.7456639999999997</v>
+        <v>6.4133120000000003</v>
       </c>
       <c r="G9" s="6">
-        <v>5.0903039999999997</v>
+        <v>4.9802239999999998</v>
       </c>
       <c r="H9" s="6">
-        <v>5.8224640000000001</v>
+        <v>5.8654719999999996</v>
       </c>
       <c r="I9" s="6">
-        <v>5.7374720000000003</v>
+        <v>4.9323079999999999</v>
       </c>
       <c r="J9" s="6">
-        <v>5.1005440000000002</v>
+        <v>5.3821440000000003</v>
       </c>
       <c r="K9" s="6">
-        <v>7.1116799999999998</v>
+        <v>5.3975039999999996</v>
       </c>
       <c r="L9" s="6">
-        <v>5.7292800000000002</v>
+        <v>5.2848639999999998</v>
       </c>
       <c r="M9" s="6">
-        <v>5.7354240000000001</v>
+        <v>5.3022720000000003</v>
       </c>
       <c r="N9" s="6">
-        <v>6.1081599999999998</v>
+        <v>5.4609920000000001</v>
       </c>
       <c r="O9" s="6">
-        <v>5.6770560000000003</v>
+        <v>5.3708799999999997</v>
       </c>
       <c r="P9" s="6">
-        <v>5.881856</v>
+        <v>5.5224320000000002</v>
       </c>
       <c r="Q9" s="6">
-        <v>5.5828480000000003</v>
+        <v>4.9684480000000004</v>
       </c>
       <c r="R9" s="6">
-        <v>4.9172479999999998</v>
+        <v>5.0728960000000001</v>
       </c>
       <c r="S9" s="6">
-        <v>4.7943680000000004</v>
+        <v>4.9991680000000001</v>
       </c>
       <c r="T9" s="6">
-        <v>3.5217407999999999</v>
+        <v>5.3585919999999998</v>
       </c>
       <c r="U9" s="6">
-        <v>5.6719359999999996</v>
+        <v>5.2008960000000002</v>
       </c>
       <c r="V9" s="6">
-        <v>5.6494080000000002</v>
+        <v>5.6330239999999998</v>
       </c>
       <c r="W9" s="5">
-        <v>4.6602240000000004</v>
+        <v>5.3340160000000001</v>
       </c>
       <c r="X9" s="6">
-        <v>21.76</v>
+        <v>5.01248</v>
       </c>
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.3">
@@ -1106,67 +1106,67 @@
       </c>
       <c r="D10" s="12">
         <f t="shared" si="0"/>
-        <v>2.3767527999999993</v>
+        <v>1.3421567999999999</v>
       </c>
       <c r="E10" s="15">
+        <v>1.3393919999999999</v>
+      </c>
+      <c r="F10" s="15">
+        <v>1.343488</v>
+      </c>
+      <c r="G10" s="15">
+        <v>1.335296</v>
+      </c>
+      <c r="H10" s="15">
+        <v>1.3056000000000001</v>
+      </c>
+      <c r="I10" s="15">
+        <v>1.3086720000000001</v>
+      </c>
+      <c r="J10" s="15">
+        <v>1.330176</v>
+      </c>
+      <c r="K10" s="15">
+        <v>1.3475839999999999</v>
+      </c>
+      <c r="L10" s="15">
+        <v>1.3895679999999999</v>
+      </c>
+      <c r="M10" s="15">
         <v>1.34144</v>
       </c>
-      <c r="F10" s="15">
-        <v>1.3342719999999999</v>
-      </c>
-      <c r="G10" s="15">
-        <v>1.343488</v>
-      </c>
-      <c r="H10" s="15">
-        <v>1.3311999999999999</v>
-      </c>
-      <c r="I10" s="15">
-        <v>1.335296</v>
-      </c>
-      <c r="J10" s="15">
-        <v>1.3076479999999999</v>
-      </c>
-      <c r="K10" s="15">
-        <v>5.7230879999999997</v>
-      </c>
-      <c r="L10" s="15">
-        <v>1.321984</v>
-      </c>
-      <c r="M10" s="15">
-        <v>1.319936</v>
-      </c>
       <c r="N10" s="15">
-        <v>1.3455360000000001</v>
+        <v>1.3393919999999999</v>
       </c>
       <c r="O10" s="15">
+        <v>1.3373440000000001</v>
+      </c>
+      <c r="P10" s="15">
+        <v>1.3086720000000001</v>
+      </c>
+      <c r="Q10" s="15">
+        <v>1.581056</v>
+      </c>
+      <c r="R10" s="15">
+        <v>1.325056</v>
+      </c>
+      <c r="S10" s="15">
+        <v>1.3271040000000001</v>
+      </c>
+      <c r="T10" s="15">
         <v>1.309696</v>
       </c>
-      <c r="P10" s="15">
-        <v>1.3178879999999999</v>
-      </c>
-      <c r="Q10" s="15">
-        <v>1.3056000000000001</v>
-      </c>
-      <c r="R10" s="15">
-        <v>8.2513919999999992</v>
-      </c>
-      <c r="S10" s="15">
-        <v>1.335296</v>
-      </c>
-      <c r="T10" s="15">
-        <v>1.311744</v>
-      </c>
       <c r="U10" s="15">
-        <v>1.3209599999999999</v>
+        <v>1.3107200000000001</v>
       </c>
       <c r="V10" s="15">
-        <v>6.36416</v>
+        <v>1.3271040000000001</v>
       </c>
       <c r="W10" s="14">
-        <v>5.9668479999999997</v>
+        <v>1.3260799999999999</v>
       </c>
       <c r="X10" s="15">
-        <v>1.3475839999999999</v>
+        <v>1.309696</v>
       </c>
     </row>
     <row r="11" spans="2:24" x14ac:dyDescent="0.3">
@@ -1178,67 +1178,67 @@
       </c>
       <c r="D11" s="12">
         <f t="shared" si="0"/>
-        <v>244946.83642879999</v>
+        <v>7.4986495999999985</v>
       </c>
       <c r="E11" s="15">
-        <v>4.9438719999999998</v>
+        <v>4.8988160000000001</v>
       </c>
       <c r="F11" s="15">
-        <v>4.8875520000000003</v>
+        <v>4.8629759999999997</v>
       </c>
       <c r="G11" s="15">
-        <v>4.8609280000000004</v>
+        <v>4.851712</v>
       </c>
       <c r="H11" s="15">
-        <v>4.8711679999999999</v>
+        <v>4.8527360000000002</v>
       </c>
       <c r="I11" s="15">
-        <v>4.9039359999999999</v>
+        <v>4.8588800000000001</v>
       </c>
       <c r="J11" s="15">
-        <v>4.8527360000000002</v>
+        <v>48.885759999999998</v>
       </c>
       <c r="K11" s="15">
-        <v>4898816</v>
+        <v>5.6954880000000001</v>
       </c>
       <c r="L11" s="15">
-        <v>4.9090559999999996</v>
+        <v>4.9223679999999996</v>
       </c>
       <c r="M11" s="15">
-        <v>4.8793600000000001</v>
+        <v>4.8865280000000002</v>
       </c>
       <c r="N11" s="15">
-        <v>6.5720320000000001</v>
+        <v>4.8988160000000001</v>
       </c>
       <c r="O11" s="15">
+        <v>4.9336320000000002</v>
+      </c>
+      <c r="P11" s="15">
+        <v>6.0098560000000001</v>
+      </c>
+      <c r="Q11" s="15">
+        <v>9.6348160000000007</v>
+      </c>
+      <c r="R11" s="15">
+        <v>4.8476160000000004</v>
+      </c>
+      <c r="S11" s="15">
         <v>4.8558079999999997</v>
       </c>
-      <c r="P11" s="15">
-        <v>4.9100799999999998</v>
-      </c>
-      <c r="Q11" s="15">
-        <v>4.8619519999999996</v>
-      </c>
-      <c r="R11" s="15">
-        <v>4.9111039999999999</v>
-      </c>
-      <c r="S11" s="15">
-        <v>1.4632959999999999</v>
-      </c>
       <c r="T11" s="15">
-        <v>4.8005120000000003</v>
+        <v>4.8680960000000004</v>
       </c>
       <c r="U11" s="15">
-        <v>22.995968000000001</v>
+        <v>4.8506879999999999</v>
       </c>
       <c r="V11" s="15">
-        <v>15.007744000000001</v>
+        <v>6.531072</v>
       </c>
       <c r="W11" s="14">
-        <v>6.3293439999999999</v>
+        <v>4.9326080000000001</v>
       </c>
       <c r="X11" s="15">
-        <v>4.912128</v>
+        <v>4.8947200000000004</v>
       </c>
     </row>
     <row r="12" spans="2:24" x14ac:dyDescent="0.3">
@@ -1250,67 +1250,67 @@
       </c>
       <c r="D12" s="12">
         <f t="shared" si="0"/>
-        <v>23.187644800000001</v>
+        <v>29.291929599999996</v>
       </c>
       <c r="E12" s="15">
-        <v>25.127935999999998</v>
+        <v>25.231359999999999</v>
       </c>
       <c r="F12" s="15">
-        <v>19.898368000000001</v>
+        <v>32.263168</v>
       </c>
       <c r="G12" s="15">
-        <v>24.908799999999999</v>
+        <v>19.837952000000001</v>
       </c>
       <c r="H12" s="15">
-        <v>26.505216000000001</v>
+        <v>23.383040000000001</v>
       </c>
       <c r="I12" s="15">
-        <v>27.089919999999999</v>
+        <v>129.32096000000001</v>
       </c>
       <c r="J12" s="15">
-        <v>20.129791999999998</v>
+        <v>24.133631999999999</v>
       </c>
       <c r="K12" s="15">
-        <v>23.088128000000001</v>
+        <v>23.306239999999999</v>
       </c>
       <c r="L12" s="15">
-        <v>22.013952</v>
+        <v>26.530816000000002</v>
       </c>
       <c r="M12" s="15">
-        <v>26.507263999999999</v>
+        <v>21.959679999999999</v>
       </c>
       <c r="N12" s="15">
-        <v>25.020416000000001</v>
+        <v>20.022272000000001</v>
       </c>
       <c r="O12" s="15">
-        <v>26.616512</v>
+        <v>20.547584000000001</v>
       </c>
       <c r="P12" s="15">
-        <v>19.715071999999999</v>
+        <v>20.936703999999999</v>
       </c>
       <c r="Q12" s="15">
-        <v>19.827711999999998</v>
+        <v>32.536575999999997</v>
       </c>
       <c r="R12" s="15">
-        <v>23.592960000000001</v>
+        <v>22.28736</v>
       </c>
       <c r="S12" s="15">
-        <v>20.105215999999999</v>
+        <v>25.58464</v>
       </c>
       <c r="T12" s="15">
-        <v>19.437567999999999</v>
+        <v>21.385216</v>
       </c>
       <c r="U12" s="15">
-        <v>19.465216000000002</v>
+        <v>21.998591999999999</v>
       </c>
       <c r="V12" s="15">
-        <v>21.899263999999999</v>
+        <v>24.767488</v>
       </c>
       <c r="W12" s="14">
-        <v>27.81184</v>
+        <v>23.649280000000001</v>
       </c>
       <c r="X12" s="15">
-        <v>24.991744000000001</v>
+        <v>26.156032</v>
       </c>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.3">
@@ -1322,67 +1322,67 @@
       </c>
       <c r="D13" s="3">
         <f t="shared" si="0"/>
-        <v>40.163209040000005</v>
+        <v>34.532044800000008</v>
       </c>
       <c r="E13" s="7">
-        <v>18.49344</v>
+        <v>19.086335999999999</v>
       </c>
       <c r="F13" s="6">
-        <v>104.78796800000001</v>
+        <v>49.784832000000002</v>
       </c>
       <c r="G13" s="6">
-        <v>18.512896000000001</v>
+        <v>113.687552</v>
       </c>
       <c r="H13" s="6">
-        <v>18.609152000000002</v>
+        <v>74.789888000000005</v>
       </c>
       <c r="I13" s="6">
-        <v>18.555904000000002</v>
+        <v>18.373632000000001</v>
       </c>
       <c r="J13" s="6">
-        <v>18.352724800000001</v>
+        <v>18.461696</v>
       </c>
       <c r="K13" s="6">
-        <v>18.558976000000001</v>
+        <v>18.663423999999999</v>
       </c>
       <c r="L13" s="6">
-        <v>107.411456</v>
+        <v>18.40128</v>
       </c>
       <c r="M13" s="6">
-        <v>98.644992000000002</v>
+        <v>103.711744</v>
       </c>
       <c r="N13" s="6">
-        <v>18.519943999999999</v>
+        <v>18.717696</v>
       </c>
       <c r="O13" s="6">
-        <v>18.332671999999999</v>
+        <v>18.458624</v>
       </c>
       <c r="P13" s="6">
-        <v>18.550784</v>
+        <v>18.585599999999999</v>
       </c>
       <c r="Q13" s="7">
-        <v>18.353152000000001</v>
+        <v>18.843648000000002</v>
       </c>
       <c r="R13" s="6">
-        <v>18.567384000000001</v>
+        <v>18.638847999999999</v>
       </c>
       <c r="S13" s="6">
-        <v>18.434048000000001</v>
+        <v>69.007360000000006</v>
       </c>
       <c r="T13" s="6">
-        <v>18.423808000000001</v>
+        <v>19.060735999999999</v>
       </c>
       <c r="U13" s="6">
-        <v>113.96608000000001</v>
+        <v>18.547712000000001</v>
       </c>
       <c r="V13" s="6">
-        <v>18.546688</v>
+        <v>18.527232000000001</v>
       </c>
       <c r="W13" s="5">
-        <v>101.30841599999999</v>
+        <v>18.848768</v>
       </c>
       <c r="X13" s="6">
-        <v>18.333696</v>
+        <v>18.444288</v>
       </c>
     </row>
     <row r="14" spans="2:24" x14ac:dyDescent="0.3">
@@ -1394,67 +1394,67 @@
       </c>
       <c r="D14" s="3">
         <f t="shared" si="0"/>
-        <v>99.769463800000025</v>
+        <v>82.730496800000012</v>
       </c>
       <c r="E14" s="6">
-        <v>255.93651199999999</v>
+        <v>97.049599999999998</v>
       </c>
       <c r="F14" s="6">
-        <v>87.656695999999997</v>
+        <v>84.787199999999999</v>
       </c>
       <c r="G14" s="6">
-        <v>96.147456000000005</v>
+        <v>77.780991999999998</v>
       </c>
       <c r="H14" s="6">
-        <v>94.605311999999998</v>
+        <v>85.803008000000005</v>
       </c>
       <c r="I14" s="6">
-        <v>94.703615999999997</v>
+        <v>78.526464000000004</v>
       </c>
       <c r="J14" s="6">
-        <v>97.310820000000007</v>
+        <v>98.018304000000001</v>
       </c>
       <c r="K14" s="6">
-        <v>87.194624000000005</v>
+        <v>94.681088000000003</v>
       </c>
       <c r="L14" s="6">
-        <v>90.769407999999999</v>
+        <v>94.454784000000004</v>
       </c>
       <c r="M14" s="6">
-        <v>91.369472000000002</v>
+        <v>73.314304000000007</v>
       </c>
       <c r="N14" s="6">
-        <v>90.890240000000006</v>
+        <v>77.133824000000004</v>
       </c>
       <c r="O14" s="6">
-        <v>91.398144000000002</v>
+        <v>78.954496000000006</v>
       </c>
       <c r="P14" s="6">
-        <v>92.332031999999998</v>
+        <v>80.431104000000005</v>
       </c>
       <c r="Q14" s="6">
-        <v>88.833023999999995</v>
+        <v>80.102400000000003</v>
       </c>
       <c r="R14" s="6">
-        <v>88.444928000000004</v>
+        <v>79.840255999999997</v>
       </c>
       <c r="S14" s="6">
-        <v>91.309055999999998</v>
+        <v>79.913983999999999</v>
       </c>
       <c r="T14" s="6">
-        <v>90.742784</v>
+        <v>76.381184000000005</v>
       </c>
       <c r="U14" s="6">
-        <v>106.883072</v>
+        <v>79.888384000000002</v>
       </c>
       <c r="V14" s="6">
-        <v>97.13664</v>
+        <v>83.375103999999993</v>
       </c>
       <c r="W14" s="5">
-        <v>74.985472000000001</v>
+        <v>82.441215999999997</v>
       </c>
       <c r="X14" s="6">
-        <v>86.739968000000005</v>
+        <v>71.732240000000004</v>
       </c>
     </row>
     <row r="15" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1466,67 +1466,67 @@
       </c>
       <c r="D15" s="3">
         <f t="shared" si="0"/>
-        <v>482.33000959999998</v>
+        <v>449.88996999999989</v>
       </c>
       <c r="E15" s="6">
-        <v>458.23078400000003</v>
+        <v>475.32339200000001</v>
       </c>
       <c r="F15" s="6">
-        <v>469.76204799999999</v>
+        <v>428.241536</v>
       </c>
       <c r="G15" s="6">
-        <v>477.17273599999999</v>
+        <v>419.37407999999999</v>
       </c>
       <c r="H15" s="6">
-        <v>461.76256000000001</v>
+        <v>444.29107199999999</v>
       </c>
       <c r="I15" s="6">
-        <v>540.87372800000003</v>
+        <v>425.55801600000001</v>
       </c>
       <c r="J15" s="6">
-        <v>472.09779200000003</v>
+        <v>520.97126400000002</v>
       </c>
       <c r="K15" s="6">
-        <v>479.06815999999998</v>
+        <v>467.25324799999999</v>
       </c>
       <c r="L15" s="6">
-        <v>469.04831999999999</v>
+        <v>474.02598399999999</v>
       </c>
       <c r="M15" s="6">
-        <v>530.68492800000001</v>
+        <v>432.41574400000002</v>
       </c>
       <c r="N15" s="6">
-        <v>467.71199999999999</v>
+        <v>428.76620800000001</v>
       </c>
       <c r="O15" s="6">
-        <v>494.65241600000002</v>
+        <v>454.55052799999999</v>
       </c>
       <c r="P15" s="6">
-        <v>578.69516799999997</v>
+        <v>510.918656</v>
       </c>
       <c r="Q15" s="6">
-        <v>466.51289600000001</v>
+        <v>483.28294399999999</v>
       </c>
       <c r="R15" s="6">
-        <v>534.18803200000002</v>
+        <v>444.98719999999997</v>
       </c>
       <c r="S15" s="6">
-        <v>456.25855999999999</v>
+        <v>435.82873599999999</v>
       </c>
       <c r="T15" s="6">
-        <v>483.20614399999999</v>
+        <v>440.302592</v>
       </c>
       <c r="U15" s="6">
-        <v>465.76025600000003</v>
+        <v>434.44224000000003</v>
       </c>
       <c r="V15" s="6">
-        <v>464.78233599999999</v>
+        <v>435.68848800000001</v>
       </c>
       <c r="W15" s="5">
-        <v>415.02515199999999</v>
+        <v>433.64864</v>
       </c>
       <c r="X15" s="6">
-        <v>461.106176</v>
+        <v>407.928832</v>
       </c>
     </row>
   </sheetData>
@@ -2508,8 +2508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED0B09C2-BC0C-46B9-8D3E-67E23CFAD3D5}">
   <dimension ref="B2:X15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="X16" sqref="X16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Y19" sqref="Y19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>